<commit_message>
Added new sheet to look up Variable information for manual upload
</commit_message>
<xml_diff>
--- a/python/01-LookupTable.xlsx
+++ b/python/01-LookupTable.xlsx
@@ -5,18 +5,19 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="335" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="182">
   <si>
     <t>datalogger</t>
   </si>
@@ -475,6 +476,93 @@
   </si>
   <si>
     <t>GS3_Moisture_EC</t>
+  </si>
+  <si>
+    <t>General Name</t>
+  </si>
+  <si>
+    <t>Specific name</t>
+  </si>
+  <si>
+    <t>VariableID</t>
+  </si>
+  <si>
+    <t>ECRN-100 Precipitation</t>
+  </si>
+  <si>
+    <t>mm Precip</t>
+  </si>
+  <si>
+    <t>ECRN50_Precipitation</t>
+  </si>
+  <si>
+    <t>GS3 Moisture/Temp/EC</t>
+  </si>
+  <si>
+    <t>dS/m EC Bulk</t>
+  </si>
+  <si>
+    <t>°C Temp</t>
+  </si>
+  <si>
+    <t>m³/m³ VWC</t>
+  </si>
+  <si>
+    <t>MPS-2 Water Potential/Temp</t>
+  </si>
+  <si>
+    <t>MPS2_WaterTemp</t>
+  </si>
+  <si>
+    <t>kPa Potential</t>
+  </si>
+  <si>
+    <t>MPS2_WPot</t>
+  </si>
+  <si>
+    <t>MPS-6 Water Potential/Temp</t>
+  </si>
+  <si>
+    <t>PYR Solar Radiation</t>
+  </si>
+  <si>
+    <t>Solar W/m²</t>
+  </si>
+  <si>
+    <t>PYR_SolarRadiation</t>
+  </si>
+  <si>
+    <t>DS-2 Sonic Anemometer</t>
+  </si>
+  <si>
+    <t>m/s Wind</t>
+  </si>
+  <si>
+    <t>SONIC_WindSpeed</t>
+  </si>
+  <si>
+    <t>SRS-Ni NDVI Hemispherical</t>
+  </si>
+  <si>
+    <t>800 nm</t>
+  </si>
+  <si>
+    <t>SRS_Ni_NDVI_eighthundred</t>
+  </si>
+  <si>
+    <t>α for NDVI</t>
+  </si>
+  <si>
+    <t>SRS_Ni_NDVI_Hemi_alpha</t>
+  </si>
+  <si>
+    <t>630 nm</t>
+  </si>
+  <si>
+    <t>SRS_Ni_NDVI_sixthirty</t>
+  </si>
+  <si>
+    <t>SRS-Nr NDVI Field Stop</t>
   </si>
 </sst>
 </file>
@@ -579,23 +667,23 @@
   </sheetPr>
   <dimension ref="A1:I105"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D111" activeCellId="0" sqref="D111"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B96" activeCellId="0" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.37777777777778"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.62222222222222"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.37674418604651"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.62325581395349"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.1222222222222"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.2976744186046"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.1296296296296"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="23.6222222222222"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.8740740740741"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.1302325581395"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="23.6186046511628"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.8744186046512"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.3703703703704"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.3767441860465"/>
     <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="11"/>
   </cols>
   <sheetData>
@@ -3479,10 +3567,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.53333333333333"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.5"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.7555555555556"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.53333333333333"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.53023255813953"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.5023255813953"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.7488372093023"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.53023255813953"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3647,4 +3735,271 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.4651162790698"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="18.8697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.5023255813953"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>